<commit_message>
Update data for 22.03.2020 + changed parameters in params.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">21.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.03.2020</t>
   </si>
 </sst>
 </file>
@@ -115,6 +118,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -266,17 +270,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,6 +556,17 @@
         <v>1676</v>
       </c>
       <c r="C25" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1782</v>
+      </c>
+      <c r="C26" s="0" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated data for 23.03.2020 + fix in ploting function
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">22.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.03.2020</t>
   </si>
 </sst>
 </file>
@@ -270,13 +273,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.78"/>
@@ -568,6 +571,17 @@
       </c>
       <c r="C26" s="0" t="n">
         <v>23</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2162</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version for hospitalized patients
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -20,17 +20,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">ntot</t>
+    <t xml:space="preserve">nhos</t>
   </si>
   <si>
     <t xml:space="preserve">nicu</t>
   </si>
   <si>
+    <t xml:space="preserve">25.02.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.02.2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">27.02.2020</t>
   </si>
   <si>
@@ -107,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">23.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.03.2020</t>
   </si>
 </sst>
 </file>
@@ -139,18 +148,12 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB2B2B2"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -187,12 +190,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -205,66 +204,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB2B2B2"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -273,13 +212,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.78"/>
@@ -301,8 +240,8 @@
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>9</v>
+      <c r="B2" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -312,8 +251,8 @@
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>11</v>
+      <c r="B3" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -323,8 +262,8 @@
       <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>14</v>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -334,8 +273,8 @@
       <c r="A5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>18</v>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -345,8 +284,8 @@
       <c r="A6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>22</v>
+      <c r="B6" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -356,8 +295,8 @@
       <c r="A7" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>27</v>
+      <c r="B7" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -367,67 +306,66 @@
       <c r="A8" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>34</v>
+      <c r="B8" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>42</v>
+      <c r="B9" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>53</v>
+      <c r="B10" s="0" t="n">
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1" t="n">
-        <v>66</v>
+      <c r="B11" s="0" t="n">
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="n">
-        <v>83</v>
+      <c r="B12" s="0" t="n">
+        <v>15</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <f aca="false">B14/1.25</f>
-        <v>104</v>
+      <c r="B13" s="0" t="n">
+        <v>16</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -435,10 +373,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -446,10 +384,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>200</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -457,10 +395,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>204</v>
+        <v>36</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,10 +406,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>292</v>
+        <v>38</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -479,10 +417,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>350</v>
+        <v>43</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,10 +428,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>406</v>
+        <v>52</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,10 +439,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>508</v>
+        <v>62</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,10 +450,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>608</v>
+        <v>78</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,10 +461,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>796</v>
+        <v>110</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,10 +472,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>1210</v>
+        <v>117</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,10 +483,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>1432</v>
+        <v>118</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,10 +494,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>1676</v>
+        <v>140</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,10 +505,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>1782</v>
+        <v>152</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -578,10 +516,43 @@
         <v>28</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>2162</v>
+        <v>175</v>
       </c>
       <c r="C27" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>223</v>
+      </c>
+      <c r="C29" s="0" t="n">
         <v>41</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>266</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>